<commit_message>
JS rich text editor
</commit_message>
<xml_diff>
--- a/Projekt/Erlaubte Technologien.xlsx
+++ b/Projekt/Erlaubte Technologien.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FHNW\WEBEC\webec-2024-hs\Projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00CA3F1C-D6FF-45B3-A4D5-2D7CDE5A7E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB0DBD80-782B-4864-8393-6151B08569ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="5070" windowWidth="28800" windowHeight="15375" xr2:uid="{BF61D5BC-BE89-4295-B826-DB37A7621F43}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{BF61D5BC-BE89-4295-B826-DB37A7621F43}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -128,13 +128,14 @@
     <t>keine</t>
   </si>
   <si>
+    <t>- JS SPA-Libraries wie Vue, Svelte, React, Angular
+- Alles was einen Frontend-Build benötigt und nicht einfach direkt eingebunden werden kann.</t>
+  </si>
+  <si>
     <t>- Selber geschriebenes JavaScript
 - JS Libraries zur Darstellung von Charts und Graphen (z.B. Cytosape.js)
-- JS Libraries zur Verwendung von WebSockets</t>
-  </si>
-  <si>
-    <t>- JS SPA-Libraries wie Vue, Svelte, React, Angular
-- Alles was einen Frontend-Build benötigt und nicht einfach direkt eingebunden werden kann.</t>
+- JS Libraries zur Verwendung von WebSockets
+- JS Rich Text Editor (z.B. Quill)</t>
   </si>
 </sst>
 </file>
@@ -655,16 +656,16 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>30</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>